<commit_message>
add random generator and svm try
</commit_message>
<xml_diff>
--- a/Runs.xlsx
+++ b/Runs.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\תואר שני\למידה חישובית\תרגילי בית\Goactive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30603415-0E54-48EB-B2C6-449666603A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8548DF7-074D-493E-90E2-2B1684EAD4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1092" windowWidth="14004" windowHeight="11268" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -115,6 +116,15 @@
   </si>
   <si>
     <t>try to change weights of the algorithms</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>Add log features</t>
+  </si>
+  <si>
+    <t>Change stratified kfold to repeated k fold and increase train set</t>
   </si>
 </sst>
 </file>
@@ -433,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,7 +692,32 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>0.505</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>0.50900000000000001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>